<commit_message>
update Quality Assurance Checklist
</commit_message>
<xml_diff>
--- a/US003 - Quality Assurance Checklist v1.0.xlsx
+++ b/US003 - Quality Assurance Checklist v1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvo30\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/nguyentan_vo_dxc_com/Documents/Desktop/Code/US003/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE90FCB-5C84-4470-B634-C38424C841E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{AEE90FCB-5C84-4470-B634-C38424C841E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEA5D20B-0F95-475A-864A-1B9B3FC135AC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -386,12 +386,6 @@
     <t>validator.properties</t>
   </si>
   <si>
-    <t>log4j.xml</t>
-  </si>
-  <si>
-    <t>26/08/2022</t>
-  </si>
-  <si>
     <t>US003 - Create New Moto Policy</t>
   </si>
   <si>
@@ -450,7 +444,13 @@
     <t>/UserStory003_CreateNewMotoPolicy/src/main/resources/ds-hibernate-cfg.properties</t>
   </si>
   <si>
-    <t>/UserStory003_CreateNewMotoPolicy/src/main/resources/log4j.xml</t>
+    <t>log4j2.xml</t>
+  </si>
+  <si>
+    <t>30/09/2022</t>
+  </si>
+  <si>
+    <t>/UserStory003_CreateNewMotoPolicy/src/main/resources/log4j2.xml</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="62" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F6" s="31"/>
       <c r="G6" s="28"/>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="63" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -1814,7 +1814,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>16</v>
@@ -1828,7 +1828,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>16</v>
@@ -1842,7 +1842,7 @@
         <v>78</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>16</v>
@@ -1856,7 +1856,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="44" t="s">
         <v>16</v>
@@ -1870,7 +1870,7 @@
         <v>80</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D7" s="44" t="s">
         <v>16</v>
@@ -1884,7 +1884,7 @@
         <v>81</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D8" s="44" t="s">
         <v>16</v>
@@ -1911,7 +1911,7 @@
   </sheetPr>
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1952,7 +1952,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D4" s="59" t="s">
         <v>16</v>
@@ -1966,7 +1966,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D5" s="59" t="s">
         <v>16</v>
@@ -1980,7 +1980,7 @@
         <v>83</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="59" t="s">
         <v>16</v>
@@ -1991,10 +1991,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" s="60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>16</v>
@@ -2005,10 +2005,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" s="59" t="s">
         <v>16</v>
@@ -2217,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E0A8C1-8EC5-42D2-BAFB-C420B5C8FC7C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J9:J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2291,10 +2291,10 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I3" s="25"/>
     </row>
@@ -2318,10 +2318,10 @@
         <v>88</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I4" s="25"/>
     </row>
@@ -2333,7 +2333,7 @@
         <v>33</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>46</v>
@@ -2345,7 +2345,7 @@
         <v>88</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>111</v>
@@ -2591,15 +2591,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068073968EC026B4DBE87DD3E85715D31" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f7a1f886a19eb4d4656104787b0b142">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4928f78-8817-462b-a38c-b730d253bc3b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="725f0d8d56db4f087920445967312631" ns2:_="">
     <xsd:import namespace="c4928f78-8817-462b-a38c-b730d253bc3b"/>
@@ -2731,6 +2722,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2738,14 +2738,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB6136B-6A54-49EB-94C3-1CE33ACD540D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C58AD30-BA56-4B7C-9B75-D231FC2808A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2763,6 +2755,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB6136B-6A54-49EB-94C3-1CE33ACD540D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F67BDBB-3D91-45AE-B771-A0EA7A408106}">
   <ds:schemaRefs>

</xml_diff>